<commit_message>
refined import export with confirmation
</commit_message>
<xml_diff>
--- a/core/src/main/resources/forms/ods/export_libraries_pools.xlsx
+++ b/core/src/main/resources/forms/ods/export_libraries_pools.xlsx
@@ -354,13 +354,13 @@
     <t>Barcode Kit</t>
   </si>
   <si>
-    <t>Pool Number</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Remember to complete all cells on the left with dropdown selections</t>
   </si>
   <si>
     <t>Adaptor</t>
+  </si>
+  <si>
+    <t>Pool Name</t>
   </si>
 </sst>
 </file>
@@ -799,6 +799,73 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -814,12 +881,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -832,71 +893,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5:V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1247,7 +1247,7 @@
       <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="40"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="3"/>
@@ -1255,135 +1255,135 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="41"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" thickBot="1"/>
     <row r="4" spans="1:22" ht="15" thickBot="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="34" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="12" t="s">
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="12" t="s">
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="14"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="37"/>
     </row>
     <row r="5" spans="1:22" ht="14" customHeight="1">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="U5" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="R5" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="T5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="U5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="V5" s="21" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="6" spans="1:22" ht="15" thickBot="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="22"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="43"/>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1"/>
@@ -1414,21 +1414,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A4:F4"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="R4:V4"/>
     <mergeCell ref="S5:S6"/>
@@ -1440,6 +1425,21 @@
     <mergeCell ref="Q5:Q6"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Prepare for MISO 0.2.1 release candidate
- MISO-41: Increase dilution information in pool listing views

- MISO-46: Fix pool Ready To Run toggle checkboxes

- MISO-63: Add URL, where supported, into alert messages

- Add EntityGroup support, notably Sample groups in ProjectOverviews

- Fix Group saving

- Add ability for users to change email and own passwords (JDBC only)

- Remove specific platform Pool implementations (everything Pool<Poolable>)

- Improve sample/library import/export functionality and spreadsheets

- Enforce lazyGet for all Store implementations

- Split out unweildy editProject.jsp javascript into separate .js files

- Improve password codec support

- Fix Pool naming when creating Pools through the wizard interface
</commit_message>
<xml_diff>
--- a/core/src/main/resources/forms/ods/export_libraries_pools.xlsx
+++ b/core/src/main/resources/forms/ods/export_libraries_pools.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="19240"/>
+    <workbookView xWindow="2980" yWindow="0" windowWidth="25600" windowHeight="19240"/>
   </bookViews>
   <sheets>
     <sheet name="library_pool_export" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="116">
   <si>
     <t xml:space="preserve">PRO </t>
   </si>
@@ -354,13 +354,31 @@
     <t>Barcode Kit</t>
   </si>
   <si>
-    <t xml:space="preserve"> Remember to complete all cells on the left with dropdown selections</t>
-  </si>
-  <si>
-    <t>Adaptor</t>
-  </si>
-  <si>
     <t>Pool Name</t>
+  </si>
+  <si>
+    <t>16s V4 Indices</t>
+  </si>
+  <si>
+    <t>454 Rapid Library</t>
+  </si>
+  <si>
+    <t>Bioo NEXTflex V1 Directional RNA-Seq Indices</t>
+  </si>
+  <si>
+    <t>Nextera Dual Index</t>
+  </si>
+  <si>
+    <t>TGAC Custom Nextera 384 Index</t>
+  </si>
+  <si>
+    <t>TruSeq Single Index</t>
+  </si>
+  <si>
+    <t>Bioo NEXTflex V2 Directional RNA-Seq Indices</t>
+  </si>
+  <si>
+    <t>Adaptor (Use Barcode Tag)</t>
   </si>
 </sst>
 </file>
@@ -442,15 +460,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -720,21 +744,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -758,7 +767,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -775,14 +784,42 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="21" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="21" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
@@ -803,10 +840,61 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="3" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -815,10 +903,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -827,37 +930,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -866,41 +942,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="48">
     <cellStyle name="Excel Built-in Normal" xfId="13"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -908,12 +975,44 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -1217,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5:V6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1228,162 +1327,160 @@
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
     <col min="5" max="6" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="11" t="s">
-        <v>107</v>
-      </c>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:22" ht="15" thickBot="1">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:22" ht="15" thickBot="1"/>
     <row r="4" spans="1:22" ht="15" thickBot="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="25" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="35" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="35" t="s">
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="37"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="20"/>
     </row>
     <row r="5" spans="1:22" ht="14" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="44" t="s">
+      <c r="R5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="38" t="s">
+      <c r="S5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="T5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="40" t="s">
+      <c r="U5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="42" t="s">
-        <v>109</v>
+      <c r="V5" s="27" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15" thickBot="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="43"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="28"/>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1"/>
@@ -1395,7 +1492,6 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1410,21 +1506,10 @@
       <c r="V7" s="1"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="N12" s="11"/>
+      <c r="N12" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="N5:N6"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="J5:J6"/>
@@ -1440,6 +1525,17 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="K5:K6"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1487,10 +1583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1498,383 +1594,409 @@
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="7" t="b">
+      <c r="F1" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="7" t="b">
+      <c r="F3" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10" t="s">
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5"/>
+      <c r="B5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10" t="s">
+      <c r="F5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5"/>
+      <c r="B6" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10" t="s">
+      <c r="F6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5"/>
+      <c r="B7" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10" t="s">
+      <c r="F7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5"/>
+      <c r="B8" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="9"/>
+      <c r="F8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5"/>
+      <c r="B9" s="7"/>
       <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
+      <c r="F9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
       <c r="C10" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5"/>
+      <c r="B11" s="8"/>
       <c r="C11" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5"/>
+      <c r="B12" s="8"/>
       <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
+    <row r="13" spans="1:6">
+      <c r="A13" s="5"/>
+      <c r="B13" s="8"/>
       <c r="C13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="7"/>
-      <c r="B14" s="10"/>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5"/>
+      <c r="B14" s="8"/>
       <c r="C14" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5"/>
+      <c r="B15" s="8"/>
       <c r="C15" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
+    <row r="16" spans="1:6">
+      <c r="A16" s="5"/>
+      <c r="B16" s="8"/>
       <c r="C16" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="7"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="8"/>
       <c r="C17" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="7"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="8"/>
       <c r="C18" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="7"/>
-      <c r="B19" s="9"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="7"/>
       <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="7"/>
-      <c r="B20" s="9"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="7"/>
-      <c r="B21" s="9"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="7"/>
       <c r="C21" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="7"/>
-      <c r="B22" s="9"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="7"/>
       <c r="C22" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="7"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="7"/>
       <c r="C23" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="7"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="7"/>
       <c r="C24" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="7"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="7"/>
       <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="7"/>
-      <c r="B26" s="9"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="7"/>
       <c r="C26" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="7"/>
-      <c r="B27" s="9"/>
-      <c r="D27" s="10" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="7"/>
+      <c r="D27" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="7"/>
-      <c r="B28" s="9"/>
-      <c r="D28" s="10" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" s="7"/>
+      <c r="D28" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E28" s="7"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="7"/>
-      <c r="B29" s="9"/>
-      <c r="D29" s="10" t="s">
+      <c r="A29" s="5"/>
+      <c r="B29" s="7"/>
+      <c r="D29" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="E29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Introduce new proceed key for importing library sheet to make it into stages
</commit_message>
<xml_diff>
--- a/core/src/main/resources/forms/ods/export_libraries_pools.xlsx
+++ b/core/src/main/resources/forms/ods/export_libraries_pools.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="0" windowWidth="25600" windowHeight="19240"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="119">
   <si>
     <t xml:space="preserve">PRO </t>
   </si>
@@ -379,6 +379,97 @@
   </si>
   <si>
     <t>Adaptor (Use Barcode Tag)</t>
+  </si>
+  <si>
+    <t>Proceed Key</t>
+  </si>
+  <si>
+    <t>Refer to right</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or empty: import everything
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: import library only
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Update the library info
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: import the library dilution and pool based on the library info (Proceed)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -474,7 +565,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -766,8 +857,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -816,8 +1002,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -852,6 +1040,30 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -879,12 +1091,6 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -967,7 +1173,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="50">
     <cellStyle name="Excel Built-in Normal" xfId="13"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -991,6 +1197,7 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1013,6 +1220,7 @@
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -1314,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1330,7 +1538,7 @@
     <col min="10" max="10" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
@@ -1347,8 +1555,14 @@
         <v>21</v>
       </c>
       <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:22" ht="15" thickBot="1">
+      <c r="X1" s="19"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" ht="15" thickBot="1">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1356,133 +1570,173 @@
       <c r="E2" s="17"/>
       <c r="F2" s="11"/>
       <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:22" ht="15" thickBot="1"/>
-    <row r="4" spans="1:22" ht="15" thickBot="1">
-      <c r="A4" s="35" t="s">
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+    </row>
+    <row r="3" spans="1:29" ht="15" customHeight="1" thickBot="1">
+      <c r="X3" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="25"/>
+    </row>
+    <row r="4" spans="1:29" ht="15" customHeight="1" thickBot="1">
+      <c r="A4" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="35" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="18" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="18" t="s">
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="20"/>
-    </row>
-    <row r="5" spans="1:22" ht="14" customHeight="1">
-      <c r="A5" s="53" t="s">
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="28"/>
+    </row>
+    <row r="5" spans="1:29" ht="14" customHeight="1">
+      <c r="A5" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="40" t="s">
+      <c r="L5" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="33" t="s">
+      <c r="N5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="29" t="s">
+      <c r="Q5" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="31" t="s">
+      <c r="R5" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="S5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="23" t="s">
+      <c r="T5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="U5" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="27" t="s">
+      <c r="V5" s="21" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="15" thickBot="1">
-      <c r="A6" s="49"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="28"/>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W5" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="28"/>
+    </row>
+    <row r="6" spans="1:29" ht="15" thickBot="1">
+      <c r="A6" s="61"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="30"/>
+      <c r="AB6" s="30"/>
+      <c r="AC6" s="31"/>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1505,11 +1759,11 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:29">
       <c r="N12" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="J5:J6"/>
@@ -1525,6 +1779,8 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="K5:K6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X3:AC6"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="R4:V4"/>
     <mergeCell ref="S5:S6"/>

</xml_diff>

<commit_message>
Bootstrap ready from internal repo
</commit_message>
<xml_diff>
--- a/core/src/main/resources/forms/ods/export_libraries_pools.xlsx
+++ b/core/src/main/resources/forms/ods/export_libraries_pools.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="0" windowWidth="25600" windowHeight="19240"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="116">
   <si>
     <t xml:space="preserve">PRO </t>
   </si>
@@ -379,97 +379,6 @@
   </si>
   <si>
     <t>Adaptor (Use Barcode Tag)</t>
-  </si>
-  <si>
-    <t>Proceed Key</t>
-  </si>
-  <si>
-    <t>Refer to right</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or empty: import everything
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: import library only
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Update the library info
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: import the library dilution and pool based on the library info (Proceed)</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -565,7 +474,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -857,103 +766,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -1002,10 +816,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -1040,11 +852,31 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1053,44 +885,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1173,7 +967,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="48">
     <cellStyle name="Excel Built-in Normal" xfId="13"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1197,7 +991,6 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1220,7 +1013,6 @@
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -1522,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3:AC6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1538,7 +1330,7 @@
     <col min="10" max="10" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:22">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
@@ -1555,14 +1347,8 @@
         <v>21</v>
       </c>
       <c r="F1" s="10"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-    </row>
-    <row r="2" spans="1:29" ht="15" thickBot="1">
+    </row>
+    <row r="2" spans="1:22" ht="15" thickBot="1">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1570,173 +1356,133 @@
       <c r="E2" s="17"/>
       <c r="F2" s="11"/>
       <c r="G2" s="9"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-    </row>
-    <row r="3" spans="1:29" ht="15" customHeight="1" thickBot="1">
-      <c r="X3" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="25"/>
-    </row>
-    <row r="4" spans="1:29" ht="15" customHeight="1" thickBot="1">
-      <c r="A4" s="47" t="s">
+    </row>
+    <row r="3" spans="1:22" ht="15" thickBot="1"/>
+    <row r="4" spans="1:22" ht="15" thickBot="1">
+      <c r="A4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="47" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="32" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="32" t="s">
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="28"/>
-    </row>
-    <row r="5" spans="1:29" ht="14" customHeight="1">
-      <c r="A5" s="65" t="s">
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="20"/>
+    </row>
+    <row r="5" spans="1:22" ht="14" customHeight="1">
+      <c r="A5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="52" t="s">
+      <c r="J5" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="52" t="s">
+      <c r="L5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="50" t="s">
+      <c r="M5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="37" t="s">
+      <c r="O5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="37" t="s">
+      <c r="P5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="41" t="s">
+      <c r="Q5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="43" t="s">
+      <c r="R5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="37" t="s">
+      <c r="T5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="39" t="s">
+      <c r="U5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="21" t="s">
+      <c r="V5" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="W5" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="27"/>
-      <c r="Z5" s="27"/>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="27"/>
-      <c r="AC5" s="28"/>
-    </row>
-    <row r="6" spans="1:29" ht="15" thickBot="1">
-      <c r="A6" s="61"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="30"/>
-      <c r="AB6" s="30"/>
-      <c r="AC6" s="31"/>
-    </row>
-    <row r="7" spans="1:29">
+    </row>
+    <row r="6" spans="1:22" ht="15" thickBot="1">
+      <c r="A6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="28"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1759,11 +1505,11 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:22">
       <c r="N12" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="26">
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="J5:J6"/>
@@ -1779,8 +1525,6 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X3:AC6"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="R4:V4"/>
     <mergeCell ref="S5:S6"/>

</xml_diff>